<commit_message>
New post filter values
</commit_message>
<xml_diff>
--- a/dac-pcm1704/background/pcm1704-post-filter.xlsx
+++ b/dac-pcm1704/background/pcm1704-post-filter.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schenk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schenk/Documents/GitHub/electronic-projects/dac-pcm1704/background/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F34A18-B64F-E144-845A-1E827225367C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF708906-63E0-6D49-9EE2-0F9BABE5A9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{FE0170E5-4D66-1649-BED9-880DF8717D42}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{FE0170E5-4D66-1649-BED9-880DF8717D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -542,7 +542,7 @@
   <dimension ref="A3:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +583,7 @@
         <v>3.3E-10</v>
       </c>
       <c r="E4">
-        <f>1/(2*3.141*SQRT(A4*B4*C4*D4))</f>
+        <f t="shared" ref="E4:E9" si="0">1/(2*3.141*SQRT(A4*B4*C4*D4))</f>
         <v>22297.963566950508</v>
       </c>
     </row>
@@ -601,7 +601,7 @@
         <v>5.6000000000000003E-10</v>
       </c>
       <c r="E5">
-        <f>1/(2*3.141*SQRT(A5*B5*C5*D5))</f>
+        <f t="shared" si="0"/>
         <v>46777.045445865289</v>
       </c>
     </row>
@@ -619,7 +619,7 @@
         <v>2.7E-10</v>
       </c>
       <c r="E6">
-        <f>1/(2*3.141*SQRT(A6*B6*C6*D6))</f>
+        <f t="shared" si="0"/>
         <v>99920.882037927062</v>
       </c>
     </row>
@@ -637,7 +637,7 @@
         <v>2.1999999999999999E-10</v>
       </c>
       <c r="E7">
-        <f>1/(2*3.141*SQRT(A7*B7*C7*D7))</f>
+        <f t="shared" si="0"/>
         <v>122241.8389295972</v>
       </c>
     </row>
@@ -655,7 +655,7 @@
         <v>1.8E-10</v>
       </c>
       <c r="E8">
-        <f>1/(2*3.141*SQRT(A8*B8*C8*D8))</f>
+        <f t="shared" si="0"/>
         <v>163533.93051626935</v>
       </c>
     </row>
@@ -673,8 +673,18 @@
         <v>7.5E-11</v>
       </c>
       <c r="E9">
-        <f>1/(2*3.141*SQRT(A9*B9*C9*D9))</f>
+        <f t="shared" si="0"/>
         <v>364859.47371990286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <f>2.2/1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I10">
+        <f>560/2.2</f>
+        <v>254.54545454545453</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>